<commit_message>
Added real Excel file v3
</commit_message>
<xml_diff>
--- a/public/data/teachers.xlsx
+++ b/public/data/teachers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT Course\nextjs\next-teacher-app\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5B790F-8CB5-4FED-BFA3-4CF5173A2B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F093086-F979-4F18-8DF7-3066E0BFA108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8751F432-B474-46C5-90E1-B8FF067F0BB9}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="383">
   <si>
     <t>Sr.No.</t>
   </si>
@@ -463,9 +463,6 @@
     <t>Junior Elementary School Teacher</t>
   </si>
   <si>
-    <t>OTHER</t>
-  </si>
-  <si>
     <t>NIL</t>
   </si>
   <si>
@@ -580,9 +577,6 @@
     <t>KARACHI</t>
   </si>
   <si>
-    <t>PST (Order: No.SELD/RP-2021/Rec./PST(3457-64) Date:14-06-2022)</t>
-  </si>
-  <si>
     <t>DIRECTOR: FARNAZ RIAZ</t>
   </si>
   <si>
@@ -925,9 +919,6 @@
     <t>SLT B-14</t>
   </si>
   <si>
-    <t>other</t>
-  </si>
-  <si>
     <t xml:space="preserve">4220108043799 </t>
   </si>
   <si>
@@ -1000,9 +991,6 @@
     <t>BS PHYSICS</t>
   </si>
   <si>
-    <t>SELD/RP/-2021/Rec./JEST(11261-70) Date 7-10-22</t>
-  </si>
-  <si>
     <t>Jamshed Road, East</t>
   </si>
   <si>
@@ -1150,9 +1138,6 @@
     <t>42301-3305481-3</t>
   </si>
   <si>
-    <t>217806</t>
-  </si>
-  <si>
     <t>Ali Khan</t>
   </si>
   <si>
@@ -1168,20 +1153,30 @@
     <t>DOE</t>
   </si>
   <si>
-    <t xml:space="preserve"> No.SELD/RP-2021/Rec./PST(3457-64) DATE :14-06-2022</t>
-  </si>
-  <si>
     <t xml:space="preserve">923022054302 </t>
   </si>
   <si>
     <t xml:space="preserve">923053838204 </t>
+  </si>
+  <si>
+    <t>No.SELD/RP-2021/Rec.JEST(15921-28)    DATE:03-11-2022</t>
+  </si>
+  <si>
+    <t>SELD/RP-2021/Rec./PST(3457-64)  DATE:14-06-2022</t>
+  </si>
+  <si>
+    <t>SELD/RP/-2021/Rec./JEST(11263-70) 
+Date 7-10-22</t>
+  </si>
+  <si>
+    <t>shaukat2181967@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1196,6 +1191,15 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1231,10 +1235,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1275,8 +1280,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1561,7 +1570,9 @@
   <dimension ref="A1:Y42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="J1" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,7 +1598,7 @@
     <col min="19" max="19" width="23.140625" style="1" customWidth="1"/>
     <col min="20" max="20" width="17.28515625" style="1" customWidth="1"/>
     <col min="21" max="21" width="13.5703125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="19.28515625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="25.28515625" style="1" customWidth="1"/>
     <col min="23" max="23" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="20" style="1" customWidth="1"/>
     <col min="25" max="25" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -1985,64 +1996,64 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>75</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="L6" s="2" t="s">
         <v>339</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>343</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>70</v>
       </c>
       <c r="N6" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="R6" s="2" t="s">
         <v>344</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>348</v>
       </c>
       <c r="S6" s="2" t="s">
         <v>109</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="V6" s="2" t="s">
         <v>47</v>
@@ -2062,16 +2073,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>75</v>
@@ -2080,16 +2091,16 @@
         <v>16</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>71</v>
@@ -2101,23 +2112,23 @@
         <v>80</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="6" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="V7" s="2" t="s">
         <v>47</v>
@@ -2137,34 +2148,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C8" s="2">
         <v>10068537</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>128</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>71</v>
@@ -2172,22 +2183,24 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="2" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="S8" s="2" t="s">
         <v>94</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="U8" s="2"/>
+        <v>358</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="V8" s="2" t="s">
         <v>47</v>
       </c>
@@ -2206,34 +2219,34 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="E9" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="F9" s="2" t="s">
         <v>291</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>293</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>74</v>
       </c>
       <c r="H9" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>296</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>97</v>
@@ -2242,28 +2255,28 @@
         <v>70</v>
       </c>
       <c r="N9" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="P9" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="Q9" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>300</v>
       </c>
       <c r="R9" s="2" t="s">
         <v>51</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>301</v>
+        <v>47</v>
       </c>
       <c r="V9" s="2" t="s">
         <v>47</v>
@@ -2283,59 +2296,63 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>376</v>
+        <v>371</v>
+      </c>
+      <c r="C10" s="6">
+        <v>10052983</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="G10" s="6">
         <v>14</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="J10" s="6"/>
+        <v>378</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>382</v>
+      </c>
       <c r="K10" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="6" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="S10" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="T10" s="6" t="s">
-        <v>347</v>
-      </c>
-      <c r="U10" s="2"/>
+        <v>343</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="V10" s="2" t="s">
         <v>47</v>
       </c>
@@ -2354,16 +2371,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>107</v>
@@ -2378,19 +2395,19 @@
         <v>47</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="Q11" s="2" t="s">
         <v>107</v>
@@ -2399,7 +2416,7 @@
         <v>82</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="T11" s="2" t="s">
         <v>107</v>
@@ -2420,21 +2437,21 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>107</v>
@@ -2443,52 +2460,55 @@
         <v>116</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>186</v>
+        <v>131</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="T12" s="2" t="s">
         <v>131</v>
       </c>
+      <c r="U12" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="V12" s="2" t="s">
-        <v>47</v>
+        <v>379</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>47</v>
+        <v>107</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="Y12" s="2" t="s">
         <v>47</v>
@@ -2505,13 +2525,13 @@
         <v>11030603</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G13" s="2">
         <v>14</v>
@@ -2523,10 +2543,10 @@
         <v>47</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>47</v>
@@ -2538,7 +2558,7 @@
         <v>47</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="P13" s="2" t="s">
         <v>144</v>
@@ -2571,39 +2591,39 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>107</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="K14" s="2" t="s">
         <v>322</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>323</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>325</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2" t="s">
@@ -2613,10 +2633,10 @@
         <v>70</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>326</v>
+        <v>381</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>107</v>
@@ -2625,7 +2645,7 @@
         <v>51</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="T14" s="2" t="s">
         <v>107</v>
@@ -2651,16 +2671,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>107</v>
@@ -2669,22 +2689,22 @@
         <v>116</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I15" s="10" t="s">
         <v>47</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>54</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -2696,7 +2716,7 @@
         <v>51</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="T15" s="2" t="s">
         <v>107</v>
@@ -2779,7 +2799,7 @@
         <v>131</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="V16" s="2" t="s">
         <v>133</v>
@@ -2788,7 +2808,7 @@
         <v>107</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="Y16" s="2" t="s">
         <v>47</v>
@@ -2799,16 +2819,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>146</v>
@@ -2817,19 +2837,19 @@
         <v>116</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I17" s="10" t="s">
         <v>47</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>70</v>
@@ -2838,10 +2858,10 @@
         <v>70</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="Q17" s="2" t="s">
         <v>107</v>
@@ -2931,7 +2951,7 @@
         <v>146</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>147</v>
+        <v>65</v>
       </c>
       <c r="V18" s="2" t="s">
         <v>47</v>
@@ -2951,16 +2971,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>107</v>
@@ -2969,53 +2989,53 @@
         <v>116</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I19" s="10" t="s">
         <v>47</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q19" s="2"/>
       <c r="R19" s="2" t="s">
         <v>82</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="U19" s="2" t="s">
         <v>65</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="Y19" s="2" t="s">
         <v>47</v>
@@ -3026,16 +3046,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>107</v>
@@ -3044,16 +3064,16 @@
         <v>116</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>47</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>71</v>
@@ -3062,31 +3082,31 @@
         <v>70</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q20" s="2" t="s">
         <v>131</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="U20" s="2" t="s">
         <v>65</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="W20" s="2" t="s">
         <v>107</v>
@@ -3180,61 +3200,61 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>131</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>47</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>70</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="P22" s="2" t="s">
         <v>95</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="R22" s="2" t="s">
         <v>51</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="U22" s="2" t="s">
         <v>93</v>
@@ -3257,37 +3277,37 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>131</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I23" s="10" t="s">
         <v>47</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>70</v>
@@ -3296,22 +3316,22 @@
         <v>70</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="P23" s="2" t="s">
         <v>95</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="R23" s="2" t="s">
         <v>51</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="U23" s="2" t="s">
         <v>93</v>
@@ -3405,34 +3425,34 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>131</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>71</v>
@@ -3444,7 +3464,7 @@
         <v>47</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="P25" s="2" t="s">
         <v>95</v>
@@ -3456,7 +3476,7 @@
         <v>51</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="T25" s="2" t="s">
         <v>131</v>
@@ -3636,31 +3656,31 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>131</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="I28" s="10" t="s">
         <v>47</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>85</v>
@@ -3675,10 +3695,10 @@
         <v>47</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q28" s="2" t="s">
         <v>131</v>
@@ -3687,7 +3707,7 @@
         <v>51</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="T28" s="2" t="s">
         <v>131</v>
@@ -3790,16 +3810,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>32</v>
@@ -3808,7 +3828,7 @@
         <v>116</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="I30" s="10" t="s">
         <v>47</v>
@@ -3817,7 +3837,7 @@
         <v>47</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="L30" s="10" t="s">
         <v>47</v>
@@ -3829,17 +3849,17 @@
         <v>47</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="P30" s="2"/>
       <c r="Q30" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="R30" s="2" t="s">
         <v>51</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="T30" s="2" t="s">
         <v>32</v>
@@ -3916,34 +3936,34 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I32" s="10" t="s">
         <v>47</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="L32" s="10" t="s">
         <v>47</v>
@@ -3952,13 +3972,13 @@
         <v>70</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="Q32" s="2" t="s">
         <v>34</v>
@@ -3967,7 +3987,7 @@
         <v>51</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="T32" s="2" t="s">
         <v>34</v>
@@ -3993,49 +4013,49 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>302</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>305</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>35</v>
       </c>
       <c r="G33" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="K33" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="H33" s="10" t="s">
+      <c r="L33" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="M33" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="I33" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="J33" s="2" t="s">
+      <c r="N33" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="K33" s="2" t="s">
+      <c r="O33" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="L33" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="M33" s="2" t="s">
+      <c r="P33" s="2" t="s">
         <v>310</v>
-      </c>
-      <c r="N33" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="O33" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="P33" s="2" t="s">
-        <v>313</v>
       </c>
       <c r="Q33" s="2" t="s">
         <v>35</v>
@@ -4125,22 +4145,22 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>37</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H35" s="10" t="s">
         <v>47</v>
@@ -4149,7 +4169,7 @@
         <v>47</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="K35" s="10" t="s">
         <v>47</v>
@@ -4164,22 +4184,22 @@
         <v>128</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="R35" s="2" t="s">
         <v>94</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="U35" s="2" t="s">
         <v>47</v>
@@ -4277,34 +4297,34 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>47</v>
@@ -4312,22 +4332,22 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="Q37" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="R37" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="R37" s="2" t="s">
-        <v>229</v>
-      </c>
       <c r="S37" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="U37" s="2" t="s">
         <v>47</v>
@@ -4731,7 +4751,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J10" r:id="rId1" xr:uid="{5E0D5FC2-3383-4092-843C-4AF7A4559513}"/>
+  </hyperlinks>
   <pageMargins left="0.28999999999999998" right="0.24" top="0.51" bottom="0.45" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" scale="37" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="5" scale="37" fitToHeight="0" orientation="landscape" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added real Excel file v4
</commit_message>
<xml_diff>
--- a/public/data/teachers.xlsx
+++ b/public/data/teachers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT Course\nextjs\next-teacher-app\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F093086-F979-4F18-8DF7-3066E0BFA108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3565DC-2513-4173-B3F7-EA5F9D9FA27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8751F432-B474-46C5-90E1-B8FF067F0BB9}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="412">
   <si>
     <t>Sr.No.</t>
   </si>
@@ -106,9 +106,6 @@
     <t>P.S.T</t>
   </si>
   <si>
-    <t>Mst. Zamarud</t>
-  </si>
-  <si>
     <t>Mst. Nusrat Jahan</t>
   </si>
   <si>
@@ -121,54 +118,21 @@
     <t>Senior Clerk</t>
   </si>
   <si>
-    <t>Mr. Iqbal</t>
-  </si>
-  <si>
     <t>Junior Clerk</t>
   </si>
   <si>
     <t>Lab Attendant</t>
   </si>
   <si>
-    <t>Mr. Shakeel Alam</t>
-  </si>
-  <si>
-    <t>Mr. Muhammad Naseem</t>
-  </si>
-  <si>
-    <t>Naib-Qasid</t>
-  </si>
-  <si>
-    <t>Mr. Muhammad Saleem</t>
-  </si>
-  <si>
-    <t>Mr. Syed Arshad Ali</t>
-  </si>
-  <si>
-    <t>Mr. Usman</t>
-  </si>
-  <si>
-    <t>Mst. Shakuntala</t>
-  </si>
-  <si>
     <t>Sweeper</t>
   </si>
   <si>
-    <t>Mr. Rajesh</t>
-  </si>
-  <si>
-    <t>Mr. Shahnawaz Ahmed</t>
-  </si>
-  <si>
     <t>Water Man</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>SIBA TESTING SERVICE</t>
-  </si>
-  <si>
     <t>Early Childhood Teacher (ECT)</t>
   </si>
   <si>
@@ -577,9 +541,6 @@
     <t>KARACHI</t>
   </si>
   <si>
-    <t>DIRECTOR: FARNAZ RIAZ</t>
-  </si>
-  <si>
     <t>B.E (Electronics)</t>
   </si>
   <si>
@@ -742,9 +703,6 @@
     <t>Naib Qasid</t>
   </si>
   <si>
-    <t>SN - Sindh (likely Korangi Karachi)</t>
-  </si>
-  <si>
     <t>SDEO Landhi/Korangi, District East, Karachi</t>
   </si>
   <si>
@@ -925,9 +883,6 @@
     <t>11104824</t>
   </si>
   <si>
-    <t>Mr. Mohsin Mir Abbasi</t>
-  </si>
-  <si>
     <t>Mir Muhammad Abbasi</t>
   </si>
   <si>
@@ -1145,12 +1100,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>8-10-1993</t>
-  </si>
-  <si>
-    <t>DOE</t>
   </si>
   <si>
     <t xml:space="preserve">923022054302 </t>
@@ -1170,13 +1119,151 @@
   </si>
   <si>
     <t>shaukat2181967@gmail.com</t>
+  </si>
+  <si>
+    <t>SHAHID ZAMAN</t>
+  </si>
+  <si>
+    <t>No.DEO/SOUTH/SEC.-MALE/(5267-70)/93, Dated: 3-10-1993</t>
+  </si>
+  <si>
+    <t>DEO, M Moosa Balouch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4200099746856 </t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4230164342005 </t>
+  </si>
+  <si>
+    <t>Ramji</t>
+  </si>
+  <si>
+    <t>Shahnawaz Ahmed</t>
+  </si>
+  <si>
+    <t>Rajesh</t>
+  </si>
+  <si>
+    <t>Shakuntala</t>
+  </si>
+  <si>
+    <t>Syed Arshad Ali</t>
+  </si>
+  <si>
+    <t>Muhammad Naseem</t>
+  </si>
+  <si>
+    <t>Shakeel Alam</t>
+  </si>
+  <si>
+    <t>Mohsin Mir Abbasi</t>
+  </si>
+  <si>
+    <t>Saghir Ahmed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4210150264439 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">923126026127 </t>
+  </si>
+  <si>
+    <t>TEO/E/EDU/GC/GEN/1(198–1200)/2009, Dated: 04-11-2009</t>
+  </si>
+  <si>
+    <t>Khurshed Alam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4210187480783 </t>
+  </si>
+  <si>
+    <t>Zamarad Fatima</t>
+  </si>
+  <si>
+    <t>Ghulam Ali Abro</t>
+  </si>
+  <si>
+    <t>Primary School Teacher</t>
+  </si>
+  <si>
+    <t>0337 3165093</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>alisohan21218@gmail.com</t>
+  </si>
+  <si>
+    <t>B.Ed (AIOU)</t>
+  </si>
+  <si>
+    <t>N/A (10-11-1990)</t>
+  </si>
+  <si>
+    <t>SELD</t>
+  </si>
+  <si>
+    <t>Larkana</t>
+  </si>
+  <si>
+    <t>Usman Baig</t>
+  </si>
+  <si>
+    <t>Ahmed Baig</t>
+  </si>
+  <si>
+    <t>Sindh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4230185837545 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4320313147836 </t>
+  </si>
+  <si>
+    <t>Syed Muhammad Ali</t>
+  </si>
+  <si>
+    <t>Mohammad Iqbal</t>
+  </si>
+  <si>
+    <t>Izhar u Din</t>
+  </si>
+  <si>
+    <t>923002279577</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4230152497995 </t>
+  </si>
+  <si>
+    <t>Mohammad Saleem</t>
+  </si>
+  <si>
+    <t>Mohammad Ismail</t>
+  </si>
+  <si>
+    <t>923082660412</t>
+  </si>
+  <si>
+    <t>923111272645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4230109221903 </t>
+  </si>
+  <si>
+    <t>+923040515908</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1197,6 +1284,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1239,7 +1333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1281,6 +1375,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1570,37 +1676,36 @@
   <dimension ref="A1:Y42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
+      <selection pane="bottomLeft" activeCell="S39" sqref="S39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.7109375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="30.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="33" style="1" customWidth="1"/>
-    <col min="16" max="16" width="29.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="23.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="34.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17.28515625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="25.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20" style="1" customWidth="1"/>
+    <col min="24" max="24" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="256" width="26" style="1" customWidth="1"/>
     <col min="257" max="16384" width="9.140625" style="1"/>
@@ -1688,153 +1793,153 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="60" x14ac:dyDescent="0.25">
@@ -1842,76 +1947,76 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -1919,76 +2024,76 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="I5" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="L5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="S5" s="2" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -1996,522 +2101,522 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>346</v>
-      </c>
       <c r="E6" s="5" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="G7" s="6">
         <v>16</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="6" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="C8" s="2">
         <v>10068537</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="2" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y9" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="C10" s="6">
         <v>10052983</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>372</v>
+        <v>357</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="G10" s="6">
         <v>14</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>378</v>
+        <v>361</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>378</v>
+        <v>361</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>382</v>
+        <v>365</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
       <c r="N10" s="6"/>
-      <c r="O10" s="6" t="s">
-        <v>375</v>
+      <c r="O10" s="1" t="s">
+        <v>367</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>375</v>
+        <v>328</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="S10" s="6" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="T10" s="6" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y10" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="H11" s="10">
         <v>923009295902</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>380</v>
+        <v>363</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>185</v>
+        <v>366</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>379</v>
+        <v>362</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="45" x14ac:dyDescent="0.25">
@@ -2525,13 +2630,13 @@
         <v>11030603</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="G13" s="2">
         <v>14</v>
@@ -2540,55 +2645,55 @@
         <v>923182952965</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y13" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="45" x14ac:dyDescent="0.25">
@@ -2596,222 +2701,222 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>381</v>
+        <v>364</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y14" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y15" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="V16" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="S16" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="T16" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="U16" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="V16" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="W16" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="Y16" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="60" x14ac:dyDescent="0.25">
@@ -2819,76 +2924,76 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="45" x14ac:dyDescent="0.25">
@@ -2896,74 +3001,74 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y18" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -2971,151 +3076,151 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="Q19" s="2"/>
       <c r="R19" s="2" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="Y19" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="W20" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="Y20" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:25" ht="60" x14ac:dyDescent="0.25">
@@ -3123,76 +3228,76 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X21" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y21" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:25" ht="60" x14ac:dyDescent="0.25">
@@ -3200,76 +3305,76 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="60" x14ac:dyDescent="0.25">
@@ -3277,147 +3382,153 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="V23" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X23" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y23" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="B24" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="C24" s="2">
+        <v>10216875</v>
+      </c>
       <c r="D24" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="5"/>
+        <v>386</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="F24" s="2" t="s">
-        <v>27</v>
+        <v>388</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>47</v>
+        <v>319</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>47</v>
+        <v>389</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>47</v>
+        <v>390</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>47</v>
+        <v>391</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>47</v>
+        <v>392</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>47</v>
+        <v>390</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>47</v>
+        <v>155</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>47</v>
+        <v>393</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>47</v>
+        <v>394</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>47</v>
+        <v>234</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>47</v>
+        <v>395</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>47</v>
+        <v>234</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X24" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y24" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:25" ht="60" x14ac:dyDescent="0.25">
@@ -3425,384 +3536,384 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>131</v>
+        <v>234</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="T25" s="2" t="s">
-        <v>131</v>
+        <v>234</v>
       </c>
       <c r="U25" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="V25" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X25" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y25" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="T26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="U26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y26" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="T27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="U27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y27" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="U28" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="V28" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W28" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X28" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y28" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="O29" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="U29" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="P29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q29" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="R29" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="S29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="T29" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="U29" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="V29" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W29" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X29" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y29" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:25" ht="45" x14ac:dyDescent="0.25">
@@ -3810,334 +3921,367 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>377</v>
+        <v>360</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M30" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="N30" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="P30" s="2"/>
       <c r="Q30" s="2" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="R30" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="T30" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U30" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V30" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W30" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X30" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y30" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>47</v>
+      <c r="B31" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="C31" s="2">
+        <v>10063909</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="5"/>
+        <v>402</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>403</v>
+      </c>
       <c r="F31" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G31" s="2"/>
-      <c r="H31" s="10"/>
+        <v>31</v>
+      </c>
+      <c r="G31" s="2">
+        <v>14</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>404</v>
+      </c>
       <c r="I31" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>291</v>
+      </c>
       <c r="L31" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R31" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="T31" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="U31" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V31" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W31" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X31" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y31" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="I32" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="T32" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="U32" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V32" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W32" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X32" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y32" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>301</v>
+        <v>379</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="I33" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="L33" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="T33" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="U33" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V33" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W33" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X33" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y33" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>47</v>
+      <c r="B34" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="C34" s="2">
+        <v>10307431</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E34" s="5"/>
+        <v>378</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>384</v>
+      </c>
       <c r="F34" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G34" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>230</v>
+      </c>
       <c r="H34" s="10"/>
       <c r="I34" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="K34" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
-      <c r="R34" s="2"/>
+      <c r="Q34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="S34" s="2"/>
-      <c r="T34" s="2"/>
+      <c r="T34" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="U34" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V34" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W34" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X34" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y34" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:25" ht="45" x14ac:dyDescent="0.25">
@@ -4145,612 +4289,613 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>37</v>
+        <v>377</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="K35" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="L35" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="S35" s="2" t="s">
-        <v>240</v>
+        <v>82</v>
+      </c>
+      <c r="S35" s="10" t="s">
+        <v>398</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="U35" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V35" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W35" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X35" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y35" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>47</v>
+      <c r="B36" s="2">
+        <v>4210176288289</v>
+      </c>
+      <c r="C36" s="2">
+        <v>10055266</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>39</v>
+        <v>406</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>47</v>
+        <v>407</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G36" s="2"/>
+        <v>226</v>
+      </c>
+      <c r="G36" s="2">
+        <v>2</v>
+      </c>
       <c r="H36" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="L36" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M36" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="N36" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O36" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="P36" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Q36" s="10" t="s">
-        <v>47</v>
+        <v>226</v>
       </c>
       <c r="R36" s="10" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="S36" s="10" t="s">
-        <v>47</v>
+        <v>398</v>
       </c>
       <c r="T36" s="10" t="s">
-        <v>47</v>
+        <v>226</v>
       </c>
       <c r="U36" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V36" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W36" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X36" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y36" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="S37" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="T37" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="T37" s="2" t="s">
-        <v>225</v>
-      </c>
       <c r="U37" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V37" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W37" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X37" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y37" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>47</v>
+      <c r="B38" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="C38" s="2">
+        <v>10079348</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>40</v>
+        <v>376</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>47</v>
+        <v>401</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>47</v>
+        <v>226</v>
+      </c>
+      <c r="G38" s="2">
+        <v>2</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="I38" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>47</v>
+        <v>194</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>47</v>
+        <v>212</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>47</v>
+        <v>214</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="T38" s="2" t="s">
-        <v>47</v>
+        <v>398</v>
+      </c>
+      <c r="T38" s="10" t="s">
+        <v>226</v>
       </c>
       <c r="U38" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V38" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W38" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X38" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y38" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>47</v>
+      <c r="B39" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="C39" s="2">
+        <v>10307370</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>41</v>
+        <v>396</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>47</v>
+        <v>397</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>47</v>
+        <v>226</v>
+      </c>
+      <c r="G39" s="2">
+        <v>1</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>47</v>
+        <v>226</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>47</v>
+        <v>214</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="T39" s="2" t="s">
-        <v>47</v>
+        <v>398</v>
+      </c>
+      <c r="T39" s="10" t="s">
+        <v>226</v>
       </c>
       <c r="U39" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V39" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W39" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X39" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y39" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>47</v>
+      <c r="B40" s="17" t="s">
+        <v>369</v>
+      </c>
+      <c r="C40" s="2">
+        <v>10752443</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>47</v>
-      </c>
+        <v>375</v>
+      </c>
+      <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>47</v>
+        <v>34</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>370</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>47</v>
+        <v>214</v>
       </c>
       <c r="S40" s="2" t="s">
-        <v>47</v>
+        <v>398</v>
       </c>
       <c r="T40" s="2" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="U40" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V40" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W40" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X40" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y40" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>47</v>
+      <c r="B41" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="C41" s="18">
+        <v>10742242</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>47</v>
+        <v>374</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>372</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>47</v>
+        <v>34</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>409</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="O41" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="O41" s="16">
+        <v>41016</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>47</v>
+        <v>214</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
       <c r="T41" s="2" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="U41" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V41" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W41" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X41" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y41" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>47</v>
+      <c r="B42" s="10" t="s">
+        <v>381</v>
+      </c>
+      <c r="C42" s="18">
+        <v>10676901</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>45</v>
+        <v>373</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>47</v>
+        <v>380</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>382</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="O42" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="O42" s="16" t="s">
+        <v>383</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="R42" s="2" t="s">
-        <v>47</v>
+        <v>214</v>
       </c>
       <c r="S42" s="2" t="s">
-        <v>47</v>
+        <v>235</v>
       </c>
       <c r="T42" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="U42" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="V42" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="W42" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="X42" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Y42" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J10" r:id="rId1" xr:uid="{5E0D5FC2-3383-4092-843C-4AF7A4559513}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Teacher data updated V5
</commit_message>
<xml_diff>
--- a/public/data/teachers.xlsx
+++ b/public/data/teachers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT Course\nextjs\next-teacher-app\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3565DC-2513-4173-B3F7-EA5F9D9FA27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785C6CD7-54C1-4908-A71B-CED3519A159C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8751F432-B474-46C5-90E1-B8FF067F0BB9}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="423">
   <si>
     <t>Sr.No.</t>
   </si>
@@ -100,18 +100,6 @@
     <t>Dr. Tanveer Jabeen</t>
   </si>
   <si>
-    <t>Campus Head (B-18)</t>
-  </si>
-  <si>
-    <t>P.S.T</t>
-  </si>
-  <si>
-    <t>Mst. Nusrat Jahan</t>
-  </si>
-  <si>
-    <t>Mst. Uroosa Nisar</t>
-  </si>
-  <si>
     <t>Mst. Nabia Naeem</t>
   </si>
   <si>
@@ -148,9 +136,6 @@
     <t>DSE/ES&amp;HS/RP-2017/Rec/ECT(2140-44)</t>
   </si>
   <si>
-    <t>_</t>
-  </si>
-  <si>
     <t>M.Ed. Diploma in Early Childhood Education</t>
   </si>
   <si>
@@ -226,9 +211,6 @@
     <t xml:space="preserve">4210117252670 </t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>Karachi-Central</t>
   </si>
   <si>
@@ -250,9 +232,6 @@
     <t>+923152706966</t>
   </si>
   <si>
-    <t>BPS-17</t>
-  </si>
-  <si>
     <t>Javed Akhtar</t>
   </si>
   <si>
@@ -289,9 +268,6 @@
     <t>+923313162115</t>
   </si>
   <si>
-    <t>HST 16</t>
-  </si>
-  <si>
     <t>Jaffer Ali</t>
   </si>
   <si>
@@ -409,12 +385,6 @@
     <t>Masters in Public Administration</t>
   </si>
   <si>
-    <t>B.Ed in progress</t>
-  </si>
-  <si>
-    <t>Merit</t>
-  </si>
-  <si>
     <t>SELD/ RP-2021/Rec/JEST(25801-08) Dated: 21-12-2022</t>
   </si>
   <si>
@@ -481,21 +451,12 @@
     <t>East Karachi</t>
   </si>
   <si>
-    <t>DEO: Yar Muhammad Baladi</t>
-  </si>
-  <si>
     <t>No.SELD/RP-2022/Rec./PST(4482-86) Date:13-04-2022</t>
   </si>
   <si>
-    <t>Women</t>
-  </si>
-  <si>
     <t>B.Sc.</t>
   </si>
   <si>
-    <t>zainabanir9221@gmail.com</t>
-  </si>
-  <si>
     <t>+923012267534</t>
   </si>
   <si>
@@ -742,9 +703,6 @@
     <t>+923213879984</t>
   </si>
   <si>
-    <t>BPS-12</t>
-  </si>
-  <si>
     <t>Shamshad ul Mulk</t>
   </si>
   <si>
@@ -820,9 +778,6 @@
     <t>Sindh Karachi</t>
   </si>
   <si>
-    <t>Junior Clerk BPS-05</t>
-  </si>
-  <si>
     <t>First Appointment: 15.07.1992 as Junior Clerk BPS-05; Promoted on 02.12.2021</t>
   </si>
   <si>
@@ -865,9 +820,6 @@
     <t>B.A</t>
   </si>
   <si>
-    <t>Woman</t>
-  </si>
-  <si>
     <t>29-09-1993 order no:(281-294)/92</t>
   </si>
   <si>
@@ -919,9 +871,6 @@
     <t>Abdul Ghaffar Siddiqui</t>
   </si>
   <si>
-    <t>Junior School Elementary Teacher (JEST)</t>
-  </si>
-  <si>
     <t>sufyansiddiqui67@gmail.com</t>
   </si>
   <si>
@@ -934,9 +883,6 @@
     <t>Kaleem Ullah</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
     <t>+923353791659</t>
   </si>
   <si>
@@ -979,9 +925,6 @@
     <t>Iqbal Masih</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
     <t>+923478288321</t>
   </si>
   <si>
@@ -997,9 +940,6 @@
     <t>M.Ed Administration</t>
   </si>
   <si>
-    <t>Woman, Minority, Christian</t>
-  </si>
-  <si>
     <t>DOE/SEC:&amp;H:SEC:(F)/(351_353)/14 Dated 21.10.14</t>
   </si>
   <si>
@@ -1114,10 +1054,6 @@
     <t>SELD/RP-2021/Rec./PST(3457-64)  DATE:14-06-2022</t>
   </si>
   <si>
-    <t>SELD/RP/-2021/Rec./JEST(11263-70) 
-Date 7-10-22</t>
-  </si>
-  <si>
     <t>shaukat2181967@gmail.com</t>
   </si>
   <si>
@@ -1187,9 +1123,6 @@
     <t>Ghulam Ali Abro</t>
   </si>
   <si>
-    <t>Primary School Teacher</t>
-  </si>
-  <si>
     <t>0337 3165093</t>
   </si>
   <si>
@@ -1202,9 +1135,6 @@
     <t>B.Ed (AIOU)</t>
   </si>
   <si>
-    <t>N/A (10-11-1990)</t>
-  </si>
-  <si>
     <t>SELD</t>
   </si>
   <si>
@@ -1257,6 +1187,108 @@
   </si>
   <si>
     <t>+923040515908</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4240104136104 </t>
+  </si>
+  <si>
+    <t>+923321305373</t>
+  </si>
+  <si>
+    <t>Uroosa Nisar</t>
+  </si>
+  <si>
+    <t>Rasheed Ahmed Memon</t>
+  </si>
+  <si>
+    <t>BPS - 14</t>
+  </si>
+  <si>
+    <t>unisar772@gmail.com</t>
+  </si>
+  <si>
+    <t>BA LLB</t>
+  </si>
+  <si>
+    <t>SELD/RP-2021/Rec./PST(16137-44) 03 Nov 2022</t>
+  </si>
+  <si>
+    <t>Directorate of School Education</t>
+  </si>
+  <si>
+    <t>SELD/RP/-2021/Rec./JEST(11263-70) Date 7-10-22</t>
+  </si>
+  <si>
+    <t>No. SDEO(G)/91-92/ Ratodero  dt 10-11-1990</t>
+  </si>
+  <si>
+    <t>Minority, Christian</t>
+  </si>
+  <si>
+    <t>zainabamir9221@gmail.com</t>
+  </si>
+  <si>
+    <t>.Abida Lodhi PSS</t>
+  </si>
+  <si>
+    <t>Nusrat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nabi Hassan </t>
+  </si>
+  <si>
+    <t>nusratjahan31118@gmail.con</t>
+  </si>
+  <si>
+    <t>23-A /1996</t>
+  </si>
+  <si>
+    <t>sub divisional educational office</t>
+  </si>
+  <si>
+    <t>west</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nill </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4210167987784 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campus Head </t>
+  </si>
+  <si>
+    <t>(B-18)</t>
+  </si>
+  <si>
+    <t>+923112508437</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>PHD</t>
+  </si>
+  <si>
+    <t>No. DSE/Admin-D/22-26/88 dated 03-01-88</t>
+  </si>
+  <si>
+    <t>923701018359</t>
+  </si>
+  <si>
+    <t>GBSS/N/1721-23/90, 08/10/90</t>
+  </si>
+  <si>
+    <t>Central, Khi, Sindh</t>
+  </si>
+  <si>
+    <t>DOE/ELE/M/REC/(77-80)/2012 dated 30-05-2012-</t>
+  </si>
+  <si>
+    <t>DOE Elementary (Male), Karachi</t>
+  </si>
+  <si>
+    <t>Gulbarg (Town), District Central</t>
   </si>
 </sst>
 </file>
@@ -1333,7 +1365,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1389,6 +1421,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1676,9 +1729,9 @@
   <dimension ref="A1:Y42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="S39" sqref="S39"/>
+      <selection pane="bottomLeft" activeCell="J34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1696,14 +1749,14 @@
     <col min="11" max="11" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="34.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="54.85546875" style="1" customWidth="1"/>
     <col min="16" max="16" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17.28515625" style="1" customWidth="1"/>
     <col min="21" max="21" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="44.7109375" style="1" customWidth="1"/>
     <col min="23" max="23" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -1788,81 +1841,81 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>36</v>
+      <c r="B2" s="10" t="s">
+        <v>389</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>411</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>36</v>
+        <v>412</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>36</v>
+        <v>390</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>36</v>
+        <v>415</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1870,76 +1923,76 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="60" x14ac:dyDescent="0.25">
@@ -1947,153 +2000,153 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>87</v>
+        <v>32</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>80</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="S5" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="M5" s="2" t="s">
+      <c r="T5" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="U5" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -2101,76 +2154,76 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>319</v>
+        <v>57</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>320</v>
+        <v>301</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>321</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>322</v>
+        <v>302</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>303</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>323</v>
+        <v>304</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>324</v>
+        <v>305</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>325</v>
+        <v>400</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -2178,74 +2231,74 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>349</v>
+        <v>329</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>344</v>
+        <v>324</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>345</v>
+        <v>325</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" s="6">
-        <v>16</v>
+        <v>58</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>352</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>348</v>
+        <v>332</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>328</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>347</v>
+        <v>327</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="6" t="s">
-        <v>354</v>
+        <v>334</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -2253,70 +2306,74 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>336</v>
+        <v>316</v>
       </c>
       <c r="C8" s="2">
         <v>10068537</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>337</v>
+        <v>317</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="I8" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>339</v>
-      </c>
       <c r="J8" s="2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
+        <v>54</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="O8" s="2" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="2" t="s">
-        <v>341</v>
+        <v>321</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -2324,151 +2381,153 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>279</v>
+        <v>32</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>264</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>281</v>
+        <v>53</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y9" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>356</v>
+        <v>336</v>
       </c>
       <c r="C10" s="6">
         <v>10052983</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>357</v>
+        <v>337</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="G10" s="6">
-        <v>14</v>
+        <v>308</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>365</v>
+        <v>344</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>359</v>
-      </c>
-      <c r="N10" s="6"/>
+        <v>339</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="O10" s="1" t="s">
-        <v>367</v>
+        <v>346</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>368</v>
+        <v>347</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="S10" s="6" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="T10" s="6" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y10" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -2476,150 +2535,156 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="H11" s="10">
         <v>923009295902</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>185</v>
+        <v>32</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>172</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
+        <v>171</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="O11" s="2" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>174</v>
+        <v>162</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>161</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>140</v>
+        <v>32</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>140</v>
+        <v>130</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>366</v>
+        <v>345</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>362</v>
+        <v>342</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2630,145 +2695,147 @@
         <v>11030603</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="G13" s="2">
-        <v>14</v>
+        <v>87</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="H13" s="10">
         <v>923182952965</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>300</v>
+        <v>32</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>283</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y13" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>304</v>
+        <v>96</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>305</v>
+        <v>287</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>306</v>
+        <v>32</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>288</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="L14" s="2"/>
+        <v>289</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="M14" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>364</v>
+        <v>398</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>308</v>
+        <v>290</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y14" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
@@ -2776,224 +2843,226 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>165</v>
+        <v>32</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>152</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="N15" s="2"/>
+        <v>130</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y15" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="O16" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="P16" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="Q16" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="R16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="S16" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H16" s="10" t="s">
+      <c r="T16" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="V16" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I16" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="S16" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="T16" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="U16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="V16" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="W16" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="Y16" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>134</v>
+        <v>87</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>206</v>
+        <v>32</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>193</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="45" x14ac:dyDescent="0.25">
@@ -3001,74 +3070,74 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="P18" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y18" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -3076,151 +3145,151 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>143</v>
+        <v>32</v>
+      </c>
+      <c r="J19" s="23" t="s">
+        <v>133</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>140</v>
+        <v>130</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="Q19" s="2"/>
       <c r="R19" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="Y19" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>157</v>
+        <v>32</v>
+      </c>
+      <c r="J20" s="23" t="s">
+        <v>401</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>155</v>
+        <v>53</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>153</v>
+        <v>402</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="W20" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="Y20" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:25" ht="60" x14ac:dyDescent="0.25">
@@ -3228,76 +3297,76 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H21" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>103</v>
-      </c>
       <c r="I21" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
+      </c>
+      <c r="J21" s="23" t="s">
+        <v>93</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X21" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y21" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:25" ht="60" x14ac:dyDescent="0.25">
@@ -3305,76 +3374,76 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>259</v>
+        <v>32</v>
+      </c>
+      <c r="J22" s="23" t="s">
+        <v>245</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>140</v>
+        <v>53</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="60" x14ac:dyDescent="0.25">
@@ -3382,153 +3451,153 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>238</v>
+        <v>32</v>
+      </c>
+      <c r="J23" s="23" t="s">
+        <v>225</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N23" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
+      </c>
+      <c r="N23" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="V23" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X23" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y23" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>400</v>
+        <v>377</v>
       </c>
       <c r="C24" s="2">
         <v>10216875</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>386</v>
+        <v>365</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>387</v>
+        <v>366</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>319</v>
+        <v>111</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>389</v>
+        <v>367</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>390</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>391</v>
+        <v>368</v>
+      </c>
+      <c r="J24" s="23" t="s">
+        <v>369</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>392</v>
+        <v>370</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="N24" s="2" t="s">
-        <v>155</v>
+        <v>53</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>394</v>
+        <v>371</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>395</v>
+        <v>372</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X24" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y24" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:25" ht="60" x14ac:dyDescent="0.25">
@@ -3536,307 +3605,305 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>248</v>
+        <v>235</v>
+      </c>
+      <c r="J25" s="23" t="s">
+        <v>234</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N25" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
+      </c>
+      <c r="N25" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="T25" s="2" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="U25" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="V25" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X25" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y25" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>27</v>
+      <c r="B26" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26" t="s">
+        <v>403</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>111</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>36</v>
+        <v>237</v>
+      </c>
+      <c r="H26" s="24" t="s">
+        <v>413</v>
+      </c>
+      <c r="I26" s="26">
+        <v>3222125432</v>
+      </c>
+      <c r="J26" s="27" t="s">
+        <v>405</v>
+      </c>
+      <c r="K26" s="25" t="s">
+        <v>414</v>
+      </c>
+      <c r="L26" s="25" t="s">
+        <v>54</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S26" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="O26" s="25" t="s">
+        <v>406</v>
+      </c>
+      <c r="P26" s="25" t="s">
+        <v>407</v>
+      </c>
+      <c r="Q26" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="R26" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="S26" s="25" t="s">
+        <v>408</v>
       </c>
       <c r="T26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="U26" s="2" t="s">
-        <v>36</v>
+        <v>221</v>
+      </c>
+      <c r="U26" s="25" t="s">
+        <v>409</v>
       </c>
       <c r="V26" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W26" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X26" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y26" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>36</v>
+      <c r="B27" s="19">
+        <v>4220176848566</v>
+      </c>
+      <c r="C27" s="18">
+        <v>11024768</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>391</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>392</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>36</v>
+        <v>111</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>393</v>
+      </c>
+      <c r="H27" s="18">
+        <v>3153503518</v>
+      </c>
+      <c r="I27" s="18">
+        <v>3232673791</v>
+      </c>
+      <c r="J27" s="21" t="s">
+        <v>394</v>
+      </c>
+      <c r="K27" s="18" t="s">
+        <v>395</v>
+      </c>
+      <c r="L27" s="18" t="s">
+        <v>131</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="U27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V27" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
+      </c>
+      <c r="N27" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="O27" s="22" t="s">
+        <v>396</v>
+      </c>
+      <c r="P27" s="22" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q27" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="R27" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="S27" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="T27" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="U27" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="V27" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="W27" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X27" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y27" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>313</v>
+        <v>295</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>304</v>
+        <v>96</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>312</v>
+        <v>294</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>311</v>
+        <v>32</v>
+      </c>
+      <c r="J28" s="23" t="s">
+        <v>293</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N28" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
+      </c>
+      <c r="N28" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="T28" s="2" t="s">
-        <v>119</v>
+        <v>291</v>
+      </c>
+      <c r="T28" s="18" t="s">
+        <v>140</v>
       </c>
       <c r="U28" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="V28" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W28" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X28" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y28" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:25" ht="60" x14ac:dyDescent="0.25">
@@ -3844,225 +3911,230 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F29" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J29" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="T29" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U29" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="P29" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q29" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R29" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="S29" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="T29" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="U29" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="V29" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W29" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X29" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y29" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="M30" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="N30" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N30" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="P30" s="2"/>
+        <v>252</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="Q30" s="2" t="s">
-        <v>266</v>
+        <v>28</v>
       </c>
       <c r="R30" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="T30" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="U30" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V30" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W30" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X30" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y30" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>405</v>
+        <v>382</v>
       </c>
       <c r="C31" s="2">
         <v>10063909</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>402</v>
+        <v>379</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>403</v>
+        <v>380</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G31" s="2">
-        <v>14</v>
+        <v>27</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>404</v>
+        <v>381</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
       <c r="L31" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N31" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>36</v>
+        <v>416</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>398</v>
+        <v>35</v>
+      </c>
+      <c r="S31" s="2" t="s">
+        <v>375</v>
       </c>
       <c r="T31" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="U31" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V31" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W31" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X31" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y31" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -4070,76 +4142,76 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="I32" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>195</v>
+        <v>32</v>
+      </c>
+      <c r="J32" s="23" t="s">
+        <v>182</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="T32" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="U32" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V32" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W32" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X32" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y32" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
@@ -4147,76 +4219,76 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>379</v>
+        <v>358</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="I33" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>290</v>
+        <v>32</v>
+      </c>
+      <c r="J33" s="23" t="s">
+        <v>274</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
       <c r="L33" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>295</v>
+        <v>279</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="T33" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="U33" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V33" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W33" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X33" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y33" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
@@ -4224,141 +4296,143 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>385</v>
+        <v>364</v>
       </c>
       <c r="C34" s="2">
         <v>10307431</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>378</v>
+        <v>357</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>384</v>
+        <v>363</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="H34" s="10"/>
       <c r="I34" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K34" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
+      <c r="N34" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
       <c r="Q34" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="S34" s="2"/>
       <c r="T34" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="U34" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V34" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W34" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X34" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y34" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>377</v>
+        <v>356</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>229</v>
+        <v>32</v>
+      </c>
+      <c r="J35" s="23" t="s">
+        <v>216</v>
       </c>
       <c r="K35" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="L35" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>82</v>
+        <v>35</v>
       </c>
       <c r="S35" s="10" t="s">
-        <v>398</v>
+        <v>419</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="U35" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V35" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W35" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X35" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y35" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
@@ -4372,70 +4446,70 @@
         <v>10055266</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>406</v>
+        <v>383</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>407</v>
+        <v>384</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="G36" s="2">
         <v>2</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>36</v>
+        <v>417</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="L36" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="M36" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="N36" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="O36" s="10" t="s">
-        <v>36</v>
+        <v>418</v>
       </c>
       <c r="P36" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Q36" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="R36" s="10" t="s">
-        <v>82</v>
+        <v>213</v>
+      </c>
+      <c r="R36" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="S36" s="10" t="s">
-        <v>398</v>
+        <v>375</v>
       </c>
       <c r="T36" s="10" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="U36" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V36" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W36" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X36" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y36" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
@@ -4443,72 +4517,76 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>218</v>
+        <v>206</v>
+      </c>
+      <c r="J37" s="23" t="s">
+        <v>205</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="O37" s="2" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>214</v>
+        <v>35</v>
       </c>
       <c r="S37" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="T37" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="T37" s="10" t="s">
-        <v>226</v>
-      </c>
       <c r="U37" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V37" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W37" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X37" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y37" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
@@ -4516,76 +4594,76 @@
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>410</v>
+        <v>387</v>
       </c>
       <c r="C38" s="2">
         <v>10079348</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>376</v>
+        <v>355</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>401</v>
+        <v>378</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="G38" s="2">
         <v>2</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>411</v>
+        <v>388</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>214</v>
+        <v>35</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>398</v>
+        <v>375</v>
       </c>
       <c r="T38" s="10" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="U38" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V38" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W38" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X38" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y38" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
@@ -4593,151 +4671,151 @@
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>399</v>
+        <v>376</v>
       </c>
       <c r="C39" s="2">
         <v>10307370</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>396</v>
+        <v>373</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>397</v>
+        <v>374</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="G39" s="2">
         <v>1</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>214</v>
+        <v>35</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>398</v>
+        <v>375</v>
       </c>
       <c r="T39" s="10" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="U39" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V39" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W39" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X39" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y39" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>369</v>
+        <v>348</v>
       </c>
       <c r="C40" s="2">
         <v>10752443</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>375</v>
+        <v>354</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>370</v>
+        <v>349</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>36</v>
+        <v>420</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>36</v>
+        <v>421</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>214</v>
+        <v>422</v>
       </c>
       <c r="S40" s="2" t="s">
-        <v>398</v>
+        <v>375</v>
       </c>
       <c r="T40" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="U40" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V40" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W40" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X40" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y40" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
@@ -4745,76 +4823,76 @@
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>371</v>
+        <v>350</v>
       </c>
       <c r="C41" s="18">
         <v>10742242</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>374</v>
+        <v>353</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>372</v>
+        <v>351</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>370</v>
+        <v>349</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>408</v>
+        <v>385</v>
       </c>
       <c r="I41" s="10" t="s">
-        <v>409</v>
+        <v>386</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="O41" s="16">
         <v>41016</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>214</v>
+        <v>35</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="T41" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="U41" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V41" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W41" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X41" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y41" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:25" ht="60" x14ac:dyDescent="0.25">
@@ -4822,84 +4900,112 @@
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>381</v>
+        <v>360</v>
       </c>
       <c r="C42" s="18">
         <v>10676901</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>380</v>
+        <v>359</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>370</v>
+        <v>349</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>382</v>
+        <v>361</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="O42" s="16" t="s">
-        <v>383</v>
+        <v>362</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="R42" s="2" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="S42" s="2" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="T42" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="U42" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V42" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="W42" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X42" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Y42" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J10" r:id="rId1" xr:uid="{5E0D5FC2-3383-4092-843C-4AF7A4559513}"/>
+    <hyperlink ref="J27" r:id="rId2" xr:uid="{6B905B0B-EAD0-4239-9CF5-115F3C4176DA}"/>
+    <hyperlink ref="J20" r:id="rId3" xr:uid="{B2CEB440-D4CF-419F-99C3-46FD7CE72980}"/>
+    <hyperlink ref="J21" r:id="rId4" xr:uid="{0ADDF287-55EF-47A8-AD51-C67C83060484}"/>
+    <hyperlink ref="J19" r:id="rId5" xr:uid="{1BD21A54-11B9-41E5-8A4B-4E85C315A0D5}"/>
+    <hyperlink ref="J18" r:id="rId6" xr:uid="{747911A7-E0F7-4896-8659-2531083A18DA}"/>
+    <hyperlink ref="J22" r:id="rId7" xr:uid="{8B62CC19-D963-4D11-8632-46FBE8EB3203}"/>
+    <hyperlink ref="J4" r:id="rId8" xr:uid="{7F45F0C0-32F5-4909-AAC9-F81B543894F5}"/>
+    <hyperlink ref="J5" r:id="rId9" xr:uid="{B2593A37-8F4C-4867-9211-80D446D5F9E5}"/>
+    <hyperlink ref="J6" r:id="rId10" xr:uid="{56F8C56D-6ECD-4875-BEE6-A6E636AF9F4C}"/>
+    <hyperlink ref="J7" r:id="rId11" xr:uid="{F3F48DA7-9C20-4AA0-B598-74CAA9F47B45}"/>
+    <hyperlink ref="J9" r:id="rId12" xr:uid="{47758CEC-8E94-4387-9662-8F90FCE2403B}"/>
+    <hyperlink ref="J12" r:id="rId13" xr:uid="{18108AFE-7480-4045-B81B-504833172517}"/>
+    <hyperlink ref="J13" r:id="rId14" xr:uid="{CEACB7FB-4224-491C-A776-B0E0ECC51FCD}"/>
+    <hyperlink ref="J37" r:id="rId15" xr:uid="{8A5F2555-10E8-467C-B2C7-95605190A8FF}"/>
+    <hyperlink ref="J35" r:id="rId16" xr:uid="{07EA6A9B-E114-4AAE-B3E2-C05C5052A4B5}"/>
+    <hyperlink ref="J33" r:id="rId17" xr:uid="{6FD14058-14FB-466A-AE38-5832DF9356C8}"/>
+    <hyperlink ref="J32" r:id="rId18" xr:uid="{A0BED852-127D-4A12-AD53-F650246DC17A}"/>
+    <hyperlink ref="J29" r:id="rId19" xr:uid="{A76E33E6-9230-4D28-AE0A-F324A3A8FC65}"/>
+    <hyperlink ref="J28" r:id="rId20" xr:uid="{BC5DB3CC-E251-4B82-AD33-25B488B26940}"/>
+    <hyperlink ref="J25" r:id="rId21" xr:uid="{ABB1453E-0BFF-4B79-824E-8FEF383E803F}"/>
+    <hyperlink ref="J23" r:id="rId22" xr:uid="{70829997-5273-4FFD-B569-217DE2A33EF3}"/>
+    <hyperlink ref="J24" r:id="rId23" xr:uid="{3004AA6F-478F-46FF-B5C6-A7021FD6C723}"/>
+    <hyperlink ref="J11" r:id="rId24" xr:uid="{2BD4D07C-5990-4FD8-9E7A-DFE697D5BFA3}"/>
+    <hyperlink ref="J14" r:id="rId25" xr:uid="{D1FF05CC-3FC7-4FE0-8B7D-A1F4F3A7E052}"/>
+    <hyperlink ref="J15" r:id="rId26" xr:uid="{C5877017-2E43-40F6-8DA3-466E0FEB4913}"/>
+    <hyperlink ref="J16" r:id="rId27" xr:uid="{2666425B-F1AF-4BBC-B2FA-5D9AA3ED5404}"/>
+    <hyperlink ref="J17" r:id="rId28" xr:uid="{A8F67140-619B-46C0-8EBD-A50A534D849A}"/>
+    <hyperlink ref="J26" r:id="rId29" xr:uid="{673FFC03-CA05-3949-9E6D-D18D71C95200}"/>
   </hyperlinks>
   <pageMargins left="0.28999999999999998" right="0.24" top="0.51" bottom="0.45" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" scale="37" fitToHeight="0" orientation="landscape" r:id="rId2"/>
+  <pageSetup paperSize="5" scale="37" fitToHeight="0" orientation="landscape" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Teacher data updated V6
</commit_message>
<xml_diff>
--- a/public/data/teachers.xlsx
+++ b/public/data/teachers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT Course\nextjs\next-teacher-app\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785C6CD7-54C1-4908-A71B-CED3519A159C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBECDCBD-702D-4660-AAF9-B0FACCB0D12D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8751F432-B474-46C5-90E1-B8FF067F0BB9}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" tabRatio="214" xr2:uid="{8751F432-B474-46C5-90E1-B8FF067F0BB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="440">
   <si>
     <t>Sr.No.</t>
   </si>
@@ -1255,21 +1255,12 @@
     <t xml:space="preserve">4210167987784 </t>
   </si>
   <si>
-    <t xml:space="preserve">Campus Head </t>
-  </si>
-  <si>
-    <t>(B-18)</t>
-  </si>
-  <si>
     <t>+923112508437</t>
   </si>
   <si>
     <t>BA</t>
   </si>
   <si>
-    <t>PHD</t>
-  </si>
-  <si>
     <t>No. DSE/Admin-D/22-26/88 dated 03-01-88</t>
   </si>
   <si>
@@ -1289,6 +1280,66 @@
   </si>
   <si>
     <t>Gulbarg (Town), District Central</t>
+  </si>
+  <si>
+    <t>Talib Hussain Alvi</t>
+  </si>
+  <si>
+    <t>HEADMISTRESS</t>
+  </si>
+  <si>
+    <t>BPS-18</t>
+  </si>
+  <si>
+    <t>tanveer_tg@hotmail.com</t>
+  </si>
+  <si>
+    <t>Ph.D.(Zoology)</t>
+  </si>
+  <si>
+    <t>M.Ed.</t>
+  </si>
+  <si>
+    <t>DOE/F/S&amp;HS/4005-08/2001 Dated 10/04/2002</t>
+  </si>
+  <si>
+    <t>HST B-16</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fakher Karim </t>
+  </si>
+  <si>
+    <t>SPSC</t>
+  </si>
+  <si>
+    <t>EDOE-CDGK/Recruitment-IV/1588/79, Dated 08-07-2011</t>
+  </si>
+  <si>
+    <t>Executive District Officer Education, City District Government Karachi</t>
+  </si>
+  <si>
+    <t>SDO/ DEF (PECHS)/58-A/1996, Dated: 12-02-1996</t>
+  </si>
+  <si>
+    <t>Sub Divisional Education Officer, District East (Female), P.E.C.H.s. Khi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">923362030431 </t>
+  </si>
+  <si>
+    <t>923322163455</t>
+  </si>
+  <si>
+    <t xml:space="preserve">923402834144 </t>
+  </si>
+  <si>
+    <t>EDOE-CDGK/R-I-IV/9708-10/2011</t>
+  </si>
+  <si>
+    <t>Executive District Officer Education, City District Government, Karachi</t>
   </si>
 </sst>
 </file>
@@ -1365,7 +1416,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1382,12 +1433,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1401,16 +1446,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1436,12 +1472,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1728,10 +1776,10 @@
   </sheetPr>
   <dimension ref="A1:Y42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="J34" sqref="A34:XFD34"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1739,18 +1787,18 @@
     <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.140625" style="1" customWidth="1"/>
     <col min="15" max="15" width="54.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33.42578125" style="1" customWidth="1"/>
     <col min="17" max="17" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -1786,10 +1834,10 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -1845,38 +1893,38 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>32</v>
+      <c r="C2" s="2">
+        <v>10055862</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>32</v>
+        <v>420</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="H2" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>390</v>
       </c>
-      <c r="I2" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>32</v>
+      <c r="I2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>32</v>
+        <v>425</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>53</v>
@@ -1885,25 +1933,25 @@
         <v>53</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>32</v>
+        <v>426</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>32</v>
+        <v>429</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>32</v>
+        <v>427</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>32</v>
+        <v>408</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>32</v>
+        <v>428</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>32</v>
+        <v>427</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>32</v>
+        <v>430</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>32</v>
@@ -1940,10 +1988,10 @@
       <c r="G3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="8" t="s">
         <v>32</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -1995,7 +2043,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2017,13 +2065,13 @@
       <c r="G4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" s="23" t="s">
+      <c r="I4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="18" t="s">
         <v>80</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -2094,13 +2142,13 @@
       <c r="G5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="I5" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="23" t="s">
+      <c r="I5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="18" t="s">
         <v>68</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -2171,13 +2219,13 @@
       <c r="G6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="J6" s="18" t="s">
         <v>303</v>
       </c>
       <c r="K6" s="2" t="s">
@@ -2230,62 +2278,62 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="20" t="s">
         <v>324</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="19" t="s">
         <v>58</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="21" t="s">
         <v>331</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="21" t="s">
         <v>332</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="22" t="s">
         <v>328</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="19" t="s">
         <v>327</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="L7" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="M7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="O7" s="6" t="s">
+      <c r="M7" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="O7" s="19" t="s">
         <v>333</v>
       </c>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6" t="s">
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="R7" s="6" t="s">
+      <c r="R7" s="19" t="s">
         <v>326</v>
       </c>
-      <c r="S7" s="6" t="s">
+      <c r="S7" s="19" t="s">
         <v>335</v>
       </c>
-      <c r="T7" s="6" t="s">
+      <c r="T7" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="U7" s="6" t="s">
+      <c r="U7" s="19" t="s">
         <v>310</v>
       </c>
       <c r="V7" s="2" t="s">
@@ -2323,10 +2371,10 @@
       <c r="G8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="8" t="s">
         <v>319</v>
       </c>
       <c r="J8" s="2" t="s">
@@ -2338,10 +2386,10 @@
       <c r="L8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="M8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="N8" s="6" t="s">
+      <c r="M8" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="N8" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O8" s="2" t="s">
@@ -2398,13 +2446,13 @@
       <c r="G9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="I9" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J9" s="23" t="s">
+      <c r="I9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="18" t="s">
         <v>264</v>
       </c>
       <c r="K9" s="2" t="s">
@@ -2416,7 +2464,7 @@
       <c r="M9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="N9" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O9" s="2" t="s">
@@ -2457,61 +2505,61 @@
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="19" t="s">
         <v>336</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="19">
         <v>10052983</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="20" t="s">
         <v>313</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="20" t="s">
         <v>337</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="19" t="s">
         <v>308</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="21" t="s">
         <v>341</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="22" t="s">
         <v>344</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="K10" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="19" t="s">
         <v>338</v>
       </c>
-      <c r="M10" s="6" t="s">
+      <c r="M10" s="19" t="s">
         <v>339</v>
       </c>
-      <c r="N10" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="O10" s="1" t="s">
+      <c r="N10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="O10" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="P10" s="6" t="s">
+      <c r="P10" s="19" t="s">
         <v>347</v>
       </c>
-      <c r="Q10" s="6" t="s">
+      <c r="Q10" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="R10" s="6" t="s">
+      <c r="R10" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="S10" s="6" t="s">
+      <c r="S10" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="T10" s="6" t="s">
+      <c r="T10" s="19" t="s">
         <v>308</v>
       </c>
       <c r="U10" s="2" t="s">
@@ -2552,13 +2600,13 @@
       <c r="G11" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="8">
         <v>923009295902</v>
       </c>
-      <c r="I11" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J11" s="23" t="s">
+      <c r="I11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="18" t="s">
         <v>172</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -2570,7 +2618,7 @@
       <c r="M11" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="N11" s="6" t="s">
+      <c r="N11" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O11" s="2" t="s">
@@ -2629,13 +2677,13 @@
       <c r="G12" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I12" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="J12" s="23" t="s">
+      <c r="J12" s="18" t="s">
         <v>161</v>
       </c>
       <c r="K12" s="2" t="s">
@@ -2647,7 +2695,7 @@
       <c r="M12" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="N12" s="6" t="s">
+      <c r="N12" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O12" s="2" t="s">
@@ -2688,7 +2736,7 @@
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="6">
         <v>4220187494713</v>
       </c>
       <c r="C13" s="2">
@@ -2706,13 +2754,13 @@
       <c r="G13" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="8">
         <v>923182952965</v>
       </c>
-      <c r="I13" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J13" s="23" t="s">
+      <c r="I13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" s="18" t="s">
         <v>283</v>
       </c>
       <c r="K13" s="2" t="s">
@@ -2724,7 +2772,7 @@
       <c r="M13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N13" s="6" t="s">
+      <c r="N13" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O13" s="2" t="s">
@@ -2783,13 +2831,13 @@
       <c r="G14" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="I14" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J14" s="23" t="s">
+      <c r="I14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J14" s="18" t="s">
         <v>288</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -2801,7 +2849,7 @@
       <c r="M14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N14" s="6" t="s">
+      <c r="N14" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O14" s="2" t="s">
@@ -2860,13 +2908,13 @@
       <c r="G15" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="I15" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J15" s="23" t="s">
+      <c r="I15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" s="18" t="s">
         <v>152</v>
       </c>
       <c r="K15" s="2" t="s">
@@ -2878,7 +2926,7 @@
       <c r="M15" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="N15" s="6" t="s">
+      <c r="N15" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O15" s="2"/>
@@ -2933,13 +2981,13 @@
       <c r="G16" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="I16" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J16" s="23" t="s">
+      <c r="I16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J16" s="18" t="s">
         <v>106</v>
       </c>
       <c r="K16" s="2" t="s">
@@ -2951,7 +2999,7 @@
       <c r="M16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N16" s="6" t="s">
+      <c r="N16" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O16" s="2" t="s">
@@ -3010,13 +3058,13 @@
       <c r="G17" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I17" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J17" s="23" t="s">
+      <c r="I17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" s="18" t="s">
         <v>193</v>
       </c>
       <c r="K17" s="2" t="s">
@@ -3028,7 +3076,7 @@
       <c r="M17" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N17" s="6" t="s">
+      <c r="N17" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O17" s="2" t="s">
@@ -3087,13 +3135,13 @@
       <c r="G18" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="I18" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J18" s="23" t="s">
+      <c r="I18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="18" t="s">
         <v>119</v>
       </c>
       <c r="K18" s="2" t="s">
@@ -3105,7 +3153,7 @@
       <c r="M18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N18" s="6" t="s">
+      <c r="N18" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O18" s="2" t="s">
@@ -3114,7 +3162,9 @@
       <c r="P18" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="Q18" s="2"/>
+      <c r="Q18" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="R18" s="2" t="s">
         <v>35</v>
       </c>
@@ -3162,13 +3212,13 @@
       <c r="G19" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="I19" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J19" s="23" t="s">
+      <c r="I19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19" s="18" t="s">
         <v>133</v>
       </c>
       <c r="K19" s="2" t="s">
@@ -3180,7 +3230,7 @@
       <c r="M19" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="N19" s="6" t="s">
+      <c r="N19" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O19" s="2" t="s">
@@ -3189,7 +3239,9 @@
       <c r="P19" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="Q19" s="2"/>
+      <c r="Q19" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="R19" s="2" t="s">
         <v>64</v>
       </c>
@@ -3237,13 +3289,13 @@
       <c r="G20" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="I20" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J20" s="23" t="s">
+      <c r="I20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J20" s="18" t="s">
         <v>401</v>
       </c>
       <c r="K20" s="2" t="s">
@@ -3255,7 +3307,7 @@
       <c r="M20" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N20" s="6" t="s">
+      <c r="N20" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O20" s="2" t="s">
@@ -3314,25 +3366,25 @@
       <c r="G21" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="J21" s="23" t="s">
+      <c r="J21" s="18" t="s">
         <v>93</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="L21" s="10" t="s">
+      <c r="L21" s="8" t="s">
         <v>32</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N21" s="6" t="s">
+      <c r="N21" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O21" s="2" t="s">
@@ -3369,7 +3421,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -3391,13 +3443,13 @@
       <c r="G22" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="I22" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J22" s="23" t="s">
+      <c r="I22" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J22" s="18" t="s">
         <v>245</v>
       </c>
       <c r="K22" s="2" t="s">
@@ -3409,7 +3461,7 @@
       <c r="M22" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N22" s="6" t="s">
+      <c r="N22" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O22" s="2" t="s">
@@ -3446,7 +3498,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -3468,13 +3520,13 @@
       <c r="G23" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="I23" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J23" s="23" t="s">
+      <c r="I23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J23" s="18" t="s">
         <v>225</v>
       </c>
       <c r="K23" s="2" t="s">
@@ -3486,7 +3538,7 @@
       <c r="M23" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N23" s="6" t="s">
+      <c r="N23" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O23" s="2" t="s">
@@ -3527,7 +3579,7 @@
       <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="8" t="s">
         <v>377</v>
       </c>
       <c r="C24" s="2">
@@ -3545,13 +3597,13 @@
       <c r="G24" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="8" t="s">
         <v>367</v>
       </c>
-      <c r="I24" s="10" t="s">
+      <c r="I24" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="J24" s="23" t="s">
+      <c r="J24" s="18" t="s">
         <v>369</v>
       </c>
       <c r="K24" s="2" t="s">
@@ -3563,7 +3615,7 @@
       <c r="M24" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N24" s="6" t="s">
+      <c r="N24" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O24" s="2" t="s">
@@ -3600,7 +3652,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -3622,13 +3674,13 @@
       <c r="G25" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="H25" s="10" t="s">
+      <c r="H25" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="I25" s="10" t="s">
+      <c r="I25" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="J25" s="23" t="s">
+      <c r="J25" s="18" t="s">
         <v>234</v>
       </c>
       <c r="K25" s="2" t="s">
@@ -3640,7 +3692,7 @@
       <c r="M25" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N25" s="6" t="s">
+      <c r="N25" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O25" s="2" t="s">
@@ -3681,14 +3733,14 @@
       <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="23" t="s">
         <v>410</v>
       </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26" t="s">
+      <c r="C26" s="24"/>
+      <c r="D26" s="24" t="s">
         <v>403</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="24" t="s">
         <v>404</v>
       </c>
       <c r="F26" s="25" t="s">
@@ -3697,17 +3749,17 @@
       <c r="G26" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="H26" s="24" t="s">
-        <v>413</v>
-      </c>
-      <c r="I26" s="26">
+      <c r="H26" s="23" t="s">
+        <v>411</v>
+      </c>
+      <c r="I26" s="24">
         <v>3222125432</v>
       </c>
-      <c r="J26" s="27" t="s">
+      <c r="J26" s="26" t="s">
         <v>405</v>
       </c>
       <c r="K26" s="25" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="L26" s="25" t="s">
         <v>54</v>
@@ -3715,7 +3767,7 @@
       <c r="M26" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N26" s="6" t="s">
+      <c r="N26" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O26" s="25" t="s">
@@ -3756,67 +3808,67 @@
       <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="14">
         <v>4220176848566</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="13">
         <v>11024768</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="15" t="s">
         <v>391</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="E27" s="15" t="s">
         <v>392</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G27" s="18" t="s">
+      <c r="G27" s="13" t="s">
         <v>393</v>
       </c>
-      <c r="H27" s="18">
+      <c r="H27" s="13">
         <v>3153503518</v>
       </c>
-      <c r="I27" s="18">
+      <c r="I27" s="13">
         <v>3232673791</v>
       </c>
-      <c r="J27" s="21" t="s">
+      <c r="J27" s="16" t="s">
         <v>394</v>
       </c>
-      <c r="K27" s="18" t="s">
+      <c r="K27" s="13" t="s">
         <v>395</v>
       </c>
-      <c r="L27" s="18" t="s">
+      <c r="L27" s="13" t="s">
         <v>131</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N27" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="O27" s="22" t="s">
+      <c r="N27" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="O27" s="17" t="s">
         <v>396</v>
       </c>
-      <c r="P27" s="22" t="s">
+      <c r="P27" s="17" t="s">
         <v>397</v>
       </c>
-      <c r="Q27" s="18" t="s">
+      <c r="Q27" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="R27" s="18" t="s">
+      <c r="R27" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="S27" s="18" t="s">
+      <c r="S27" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="T27" s="18" t="s">
+      <c r="T27" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="U27" s="18" t="s">
+      <c r="U27" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="V27" s="18" t="s">
+      <c r="V27" s="13" t="s">
         <v>32</v>
       </c>
       <c r="W27" s="2" t="s">
@@ -3851,13 +3903,13 @@
       <c r="G28" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H28" s="10" t="s">
+      <c r="H28" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="I28" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J28" s="23" t="s">
+      <c r="I28" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J28" s="18" t="s">
         <v>293</v>
       </c>
       <c r="K28" s="2" t="s">
@@ -3869,7 +3921,7 @@
       <c r="M28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N28" s="6" t="s">
+      <c r="N28" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O28" s="2" t="s">
@@ -3887,7 +3939,7 @@
       <c r="S28" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="T28" s="18" t="s">
+      <c r="T28" s="13" t="s">
         <v>140</v>
       </c>
       <c r="U28" s="2" t="s">
@@ -3928,13 +3980,13 @@
       <c r="G29" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H29" s="10" t="s">
+      <c r="H29" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="I29" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J29" s="23" t="s">
+      <c r="I29" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J29" s="18" t="s">
         <v>40</v>
       </c>
       <c r="K29" s="2" t="s">
@@ -3946,7 +3998,7 @@
       <c r="M29" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N29" s="6" t="s">
+      <c r="N29" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O29" s="2" t="s">
@@ -4005,25 +4057,25 @@
       <c r="G30" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H30" s="10" t="s">
+      <c r="H30" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="I30" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J30" s="10" t="s">
+      <c r="I30" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J30" s="8" t="s">
         <v>32</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="L30" s="10" t="s">
+      <c r="L30" s="8" t="s">
         <v>32</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N30" s="6" t="s">
+      <c r="N30" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O30" s="2" t="s">
@@ -4064,7 +4116,7 @@
       <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="8" t="s">
         <v>382</v>
       </c>
       <c r="C31" s="2">
@@ -4082,10 +4134,10 @@
       <c r="G31" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H31" s="10" t="s">
+      <c r="H31" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="I31" s="10" t="s">
+      <c r="I31" s="8" t="s">
         <v>32</v>
       </c>
       <c r="J31" s="2" t="s">
@@ -4094,20 +4146,20 @@
       <c r="K31" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="L31" s="10" t="s">
+      <c r="L31" s="8" t="s">
         <v>32</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N31" s="6" t="s">
+      <c r="N31" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>32</v>
+        <v>178</v>
       </c>
       <c r="Q31" s="2" t="s">
         <v>28</v>
@@ -4159,19 +4211,19 @@
       <c r="G32" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="H32" s="10" t="s">
+      <c r="H32" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="I32" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J32" s="23" t="s">
+      <c r="I32" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J32" s="18" t="s">
         <v>182</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="L32" s="10" t="s">
+      <c r="L32" s="8" t="s">
         <v>32</v>
       </c>
       <c r="M32" s="2" t="s">
@@ -4236,19 +4288,19 @@
       <c r="G33" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="H33" s="10" t="s">
+      <c r="H33" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="I33" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J33" s="23" t="s">
+      <c r="I33" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J33" s="18" t="s">
         <v>274</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="L33" s="10" t="s">
+      <c r="L33" s="8" t="s">
         <v>32</v>
       </c>
       <c r="M33" s="2" t="s">
@@ -4291,11 +4343,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="8" t="s">
         <v>364</v>
       </c>
       <c r="C34" s="2">
@@ -4310,28 +4362,32 @@
       <c r="F34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="G34" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J34" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="K34" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="L34" s="10" t="s">
+      <c r="H34" s="8"/>
+      <c r="I34" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K34" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L34" s="8" t="s">
         <v>32</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
+      <c r="O34" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>439</v>
+      </c>
       <c r="Q34" s="2" t="s">
         <v>29</v>
       </c>
@@ -4380,19 +4436,19 @@
       <c r="G35" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="H35" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J35" s="23" t="s">
+      <c r="H35" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J35" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="K35" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="L35" s="10" t="s">
+      <c r="K35" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L35" s="8" t="s">
         <v>32</v>
       </c>
       <c r="M35" s="2" t="s">
@@ -4413,8 +4469,8 @@
       <c r="R35" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="S35" s="10" t="s">
-        <v>419</v>
+      <c r="S35" s="8" t="s">
+        <v>416</v>
       </c>
       <c r="T35" s="2" t="s">
         <v>213</v>
@@ -4457,19 +4513,19 @@
       <c r="G36" s="2">
         <v>2</v>
       </c>
-      <c r="H36" s="10" t="s">
-        <v>417</v>
-      </c>
-      <c r="I36" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J36" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="K36" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="L36" s="10" t="s">
+      <c r="H36" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L36" s="8" t="s">
         <v>32</v>
       </c>
       <c r="M36" s="2" t="s">
@@ -4478,25 +4534,25 @@
       <c r="N36" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="O36" s="10" t="s">
-        <v>418</v>
-      </c>
-      <c r="P36" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q36" s="10" t="s">
+      <c r="O36" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="P36" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q36" s="8" t="s">
         <v>213</v>
       </c>
       <c r="R36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="S36" s="10" t="s">
+      <c r="S36" s="8" t="s">
         <v>375</v>
       </c>
-      <c r="T36" s="10" t="s">
+      <c r="T36" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="U36" s="10" t="s">
+      <c r="U36" s="8" t="s">
         <v>32</v>
       </c>
       <c r="V36" s="2" t="s">
@@ -4534,13 +4590,13 @@
       <c r="G37" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="H37" s="10" t="s">
+      <c r="H37" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="I37" s="10" t="s">
+      <c r="I37" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="J37" s="23" t="s">
+      <c r="J37" s="18" t="s">
         <v>205</v>
       </c>
       <c r="K37" s="2" t="s">
@@ -4570,7 +4626,7 @@
       <c r="S37" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="T37" s="10" t="s">
+      <c r="T37" s="8" t="s">
         <v>213</v>
       </c>
       <c r="U37" s="2" t="s">
@@ -4589,11 +4645,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="8" t="s">
         <v>387</v>
       </c>
       <c r="C38" s="2">
@@ -4611,10 +4667,10 @@
       <c r="G38" s="2">
         <v>2</v>
       </c>
-      <c r="H38" s="10" t="s">
+      <c r="H38" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="I38" s="10" t="s">
+      <c r="I38" s="8" t="s">
         <v>32</v>
       </c>
       <c r="J38" s="2" t="s">
@@ -4633,10 +4689,10 @@
         <v>53</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>32</v>
+        <v>433</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>32</v>
+        <v>434</v>
       </c>
       <c r="Q38" s="2" t="s">
         <v>199</v>
@@ -4647,7 +4703,7 @@
       <c r="S38" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="T38" s="10" t="s">
+      <c r="T38" s="8" t="s">
         <v>213</v>
       </c>
       <c r="U38" s="2" t="s">
@@ -4666,11 +4722,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="8" t="s">
         <v>376</v>
       </c>
       <c r="C39" s="2">
@@ -4688,8 +4744,8 @@
       <c r="G39" s="2">
         <v>1</v>
       </c>
-      <c r="H39" s="2" t="s">
-        <v>32</v>
+      <c r="H39" s="8" t="s">
+        <v>435</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>32</v>
@@ -4710,10 +4766,10 @@
         <v>53</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>32</v>
+        <v>431</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>32</v>
+        <v>432</v>
       </c>
       <c r="Q39" s="2" t="s">
         <v>213</v>
@@ -4724,7 +4780,7 @@
       <c r="S39" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="T39" s="10" t="s">
+      <c r="T39" s="8" t="s">
         <v>213</v>
       </c>
       <c r="U39" s="2" t="s">
@@ -4747,7 +4803,7 @@
       <c r="A40" s="2">
         <v>39</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="12" t="s">
         <v>348</v>
       </c>
       <c r="C40" s="2">
@@ -4760,11 +4816,11 @@
       <c r="F40" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G40" s="10" t="s">
+      <c r="G40" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="H40" s="2" t="s">
-        <v>32</v>
+      <c r="H40" s="8" t="s">
+        <v>437</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>32</v>
@@ -4785,16 +4841,16 @@
         <v>53</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="Q40" s="2" t="s">
         <v>30</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="S40" s="2" t="s">
         <v>375</v>
@@ -4822,10 +4878,10 @@
       <c r="A41" s="2">
         <v>40</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="C41" s="18">
+      <c r="C41" s="13">
         <v>10742242</v>
       </c>
       <c r="D41" s="5" t="s">
@@ -4837,13 +4893,13 @@
       <c r="F41" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="10" t="s">
+      <c r="G41" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="H41" s="10" t="s">
+      <c r="H41" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="I41" s="10" t="s">
+      <c r="I41" s="8" t="s">
         <v>386</v>
       </c>
       <c r="J41" s="2" t="s">
@@ -4861,7 +4917,7 @@
       <c r="N41" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="O41" s="16">
+      <c r="O41" s="11">
         <v>41016</v>
       </c>
       <c r="P41" s="2" t="s">
@@ -4895,14 +4951,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="C42" s="18">
+      <c r="C42" s="13">
         <v>10676901</v>
       </c>
       <c r="D42" s="5" t="s">
@@ -4914,10 +4970,10 @@
       <c r="F42" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G42" s="10" t="s">
+      <c r="G42" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="H42" s="10" t="s">
+      <c r="H42" s="8" t="s">
         <v>361</v>
       </c>
       <c r="I42" s="2" t="s">
@@ -4938,7 +4994,7 @@
       <c r="N42" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="O42" s="16" t="s">
+      <c r="O42" s="11" t="s">
         <v>362</v>
       </c>
       <c r="P42" s="2" t="s">
@@ -5004,8 +5060,9 @@
     <hyperlink ref="J16" r:id="rId27" xr:uid="{2666425B-F1AF-4BBC-B2FA-5D9AA3ED5404}"/>
     <hyperlink ref="J17" r:id="rId28" xr:uid="{A8F67140-619B-46C0-8EBD-A50A534D849A}"/>
     <hyperlink ref="J26" r:id="rId29" xr:uid="{673FFC03-CA05-3949-9E6D-D18D71C95200}"/>
+    <hyperlink ref="J2" r:id="rId30" xr:uid="{0AC8BAAF-B287-4398-A5BF-9BD6BB3B5308}"/>
   </hyperlinks>
   <pageMargins left="0.28999999999999998" right="0.24" top="0.51" bottom="0.45" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" scale="37" fitToHeight="0" orientation="landscape" r:id="rId30"/>
+  <pageSetup paperSize="5" scale="37" fitToHeight="0" orientation="landscape" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>